<commit_message>
Looked at Lien Doan
</commit_message>
<xml_diff>
--- a/Data/League.Chapters.xlsx
+++ b/Data/League.Chapters.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-2340" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="2" r:id="rId1"/>
     <sheet name="census_registry" sheetId="1" r:id="rId2"/>
     <sheet name="Lien Doan" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2505" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2523" uniqueCount="692">
   <si>
     <t>id</t>
   </si>
@@ -2078,6 +2079,33 @@
   </si>
   <si>
     <t>Da Minh Uy</t>
+  </si>
+  <si>
+    <t>Daminh Savio</t>
+  </si>
+  <si>
+    <t>Ra Khoi</t>
+  </si>
+  <si>
+    <t>Nguon Song</t>
+  </si>
+  <si>
+    <t>Thanh Gia</t>
+  </si>
+  <si>
+    <t>Thanh Phaolo Hanh</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Ending Index</t>
+  </si>
+  <si>
+    <t>Starting Index</t>
+  </si>
+  <si>
+    <t>Lien Doan</t>
   </si>
 </sst>
 </file>
@@ -2158,7 +2186,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2174,6 +2202,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2205,7 +2251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2271,6 +2317,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9533,7 +9582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -12031,4 +12080,252 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="20" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>691</v>
+      </c>
+      <c r="B1" t="s">
+        <v>690</v>
+      </c>
+      <c r="C1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2+1</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>482</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <f>C3-B3+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <f>C4-B4+1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
+        <v>686</v>
+      </c>
+      <c r="B5">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>55</v>
+      </c>
+      <c r="D5">
+        <f>C5-B5+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <f>C6-B6+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="s">
+        <v>686</v>
+      </c>
+      <c r="B7">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>62</v>
+      </c>
+      <c r="D7">
+        <f>C7-B7+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>485</v>
+      </c>
+      <c r="B8">
+        <v>63</v>
+      </c>
+      <c r="C8">
+        <v>73</v>
+      </c>
+      <c r="D8">
+        <f>C8-B8+1</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>685</v>
+      </c>
+      <c r="B9">
+        <v>74</v>
+      </c>
+      <c r="C9">
+        <v>87</v>
+      </c>
+      <c r="D9">
+        <f>C9-B9+1</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>684</v>
+      </c>
+      <c r="B10">
+        <v>88</v>
+      </c>
+      <c r="C10">
+        <v>99</v>
+      </c>
+      <c r="D10">
+        <f>C10-B10+1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>327</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>103</v>
+      </c>
+      <c r="D11">
+        <f>C11-B11+1</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B12">
+        <v>104</v>
+      </c>
+      <c r="C12">
+        <v>110</v>
+      </c>
+      <c r="D12">
+        <f>C12-B12+1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="B13">
+        <v>111</v>
+      </c>
+      <c r="C13">
+        <v>129</v>
+      </c>
+      <c r="D13">
+        <f>C13-B13+1</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>683</v>
+      </c>
+      <c r="B14">
+        <v>130</v>
+      </c>
+      <c r="C14">
+        <v>139</v>
+      </c>
+      <c r="D14">
+        <f>C14-B14+1</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>482</v>
+      </c>
+      <c r="B15">
+        <v>140</v>
+      </c>
+      <c r="C15">
+        <v>140</v>
+      </c>
+      <c r="D15">
+        <f>C15-B15+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <f>SUM(D2:D15)</f>
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>